<commit_message>
Add plot of average goals
</commit_message>
<xml_diff>
--- a/data/table_scrape_overview.xlsx
+++ b/data/table_scrape_overview.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stefan/Google Drive/ringarena/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stefan/GitHub/ringarena/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -259,7 +259,7 @@
     <t>http://www.sis-handball.de/default.aspx?view=AlleSpiele&amp;Liga=001517505503503501000000000000000001000</t>
   </si>
   <si>
-    <t>1. Kreislklasse</t>
+    <t>1. Kreisklasse</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Update with all matches from 2017/18
</commit_message>
<xml_diff>
--- a/data/table_scrape_overview.xlsx
+++ b/data/table_scrape_overview.xlsx
@@ -611,8 +611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="G45" sqref="G45"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -659,13 +659,13 @@
         <v>8</v>
       </c>
       <c r="D2">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E2">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="F2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G2" t="s">
         <v>11</v>
@@ -867,10 +867,10 @@
         <v>8</v>
       </c>
       <c r="D10">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="E10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -1075,10 +1075,10 @@
         <v>8</v>
       </c>
       <c r="D18">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E18">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F18">
         <v>1</v>
@@ -1283,10 +1283,10 @@
         <v>8</v>
       </c>
       <c r="D26">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E26">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="F26">
         <v>9</v>
@@ -1491,10 +1491,10 @@
         <v>8</v>
       </c>
       <c r="D34">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="E34">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F34">
         <v>3</v>
@@ -1699,13 +1699,13 @@
         <v>8</v>
       </c>
       <c r="D42">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E42">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F42">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G42" t="s">
         <v>52</v>

</xml_diff>